<commit_message>
commit on nov 8th
</commit_message>
<xml_diff>
--- a/lib/inputs.xlsx
+++ b/lib/inputs.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14850" windowHeight="7185"/>
+    <workbookView windowWidth="28695" windowHeight="13020" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginData" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLoginData" sheetId="2" r:id="rId2"/>
     <sheet name="ValidResetPasswordData" sheetId="3" r:id="rId3"/>
+    <sheet name="SymmtricKeyValid" sheetId="4" r:id="rId4"/>
+    <sheet name="SymmtricKeyInvalid" sheetId="5" r:id="rId5"/>
+    <sheet name="SymmtricKeyIncorrect" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:C2"/>
@@ -17,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>UserName</t>
   </si>
@@ -59,6 +62,33 @@
   </si>
   <si>
     <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Skey</t>
+  </si>
+  <si>
+    <t>lvzuxEzFqqkNzLYQjbWA0q6E7wySlR9Z</t>
+  </si>
+  <si>
+    <t>vFROr7RbHGkpq9NGjh61Q/A2mXXZqTD4</t>
+  </si>
+  <si>
+    <t>SymmtricKeyInvalid- with valid format</t>
+  </si>
+  <si>
+    <t>BFROr7RbHGkpq9NGjh61Q/A2mXXZqTD4</t>
+  </si>
+  <si>
+    <t>SymmtricKeyIncorrect- with invalid format-number</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>xxcvbg</t>
+  </si>
+  <si>
+    <t>SymmtricKeyIncorrect- with alphabets</t>
   </si>
 </sst>
 </file>
@@ -66,9 +96,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -104,70 +134,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -180,7 +158,66 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,7 +232,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,24 +254,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,13 +278,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,25 +320,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,139 +458,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,52 +472,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,6 +511,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -525,171 +535,192 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1014,8 +1045,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1029,7 +1060,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -1069,7 +1100,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -1080,7 +1111,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -1091,10 +1122,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -1149,4 +1180,122 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="53.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="35.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>125</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
nov 11 from office
</commit_message>
<xml_diff>
--- a/lib/inputs.xlsx
+++ b/lib/inputs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13020" firstSheet="6" activeTab="9"/>
+    <workbookView windowWidth="28695" windowHeight="13020" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginData" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="ValidResearcherEmails" sheetId="9" r:id="rId9"/>
     <sheet name="InvalidResearcherEmails" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>UserName</t>
   </si>
@@ -94,74 +94,71 @@
     <t>SymmtricKeyIncorrect- with alphabets</t>
   </si>
   <si>
-    <t>Email ID's</t>
-  </si>
-  <si>
-    <t>karthik.m@dreamorbit.com</t>
+    <t>Email ID</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Registered, but not even logged in once</t>
-  </si>
-  <si>
-    <t>karthik.nonreg@dreamorbit.com</t>
-  </si>
-  <si>
-    <t>Not registered user</t>
-  </si>
-  <si>
-    <t>Empty data</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>Wrong Email ID format</t>
-  </si>
-  <si>
-    <t>Email ID</t>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>karthik.m+auto3@dreamorbit.com</t>
   </si>
   <si>
     <t>ChiefReseracher</t>
   </si>
   <si>
+    <t>karthik.m+1@dreamorbit.com</t>
+  </si>
+  <si>
     <t>Researcher</t>
-  </si>
-  <si>
-    <t>karthik.m+81@dreamorbit.com</t>
-  </si>
-  <si>
-    <t>Expired password user</t>
   </si>
   <si>
     <t xml:space="preserve">PWD- 0NmxX,YN
 </t>
   </si>
   <si>
-    <t>karthik.m+auto3@dreamorbit.com</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
     <t>R6lD7ItuUMx+oRpfy0VcwZnrAnq+jCCi</t>
   </si>
   <si>
-    <t>karthik.m+1@dreamorbit.com</t>
+    <t>Email ID's</t>
+  </si>
+  <si>
+    <t>Empty data</t>
+  </si>
+  <si>
+    <t>karthik.m@dreamorbit.com</t>
+  </si>
+  <si>
+    <t>Registered, but not even logged in once</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Wrong Email ID format</t>
+  </si>
+  <si>
+    <t>karthik.nonreg@dreamorbit.com</t>
+  </si>
+  <si>
+    <t>Not registered user</t>
+  </si>
+  <si>
+    <t>karthik.m+81@dreamorbit.com</t>
+  </si>
+  <si>
+    <t>Expired password user</t>
+  </si>
+  <si>
+    <t>res58@test1.com</t>
+  </si>
+  <si>
+    <t>res897@test2.com</t>
   </si>
   <si>
     <t>res4@test3.com</t>
-  </si>
-  <si>
-    <t>res5@test2.com</t>
-  </si>
-  <si>
-    <t>res7@test3.com</t>
-  </si>
-  <si>
-    <t>res6@test1.com</t>
   </si>
   <si>
     <t>Already existing user</t>
@@ -180,7 +177,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +192,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,29 +216,344 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -227,29 +561,314 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -511,30 +1130,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -543,55 +1162,57 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="mailto:venkatesh.n@dreamorbit.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="venkatesh.n@dreamorbit.com" tooltip="mailto:venkatesh.n@dreamorbit.com"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="1" max="1" width="29.552380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>42</v>
+      <c r="A2" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -599,42 +1220,44 @@
         <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" display="res4@test3.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="auto@hm.c"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.1047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -645,7 +1268,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -656,10 +1279,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -668,32 +1291,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" display="karthik.ds@dreamorbit.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="karthik.mns@dreamorbit.com"/>
+    <hyperlink ref="A4" r:id="rId1" display="karthik.ds@dreamorbit.com"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -709,25 +1334,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="53.44140625" customWidth="1"/>
+    <col min="1" max="1" width="53.4380952380952" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -737,26 +1364,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35.552380952381" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -768,31 +1397,33 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -800,15 +1431,15 @@
       <c r="A2">
         <v>125</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -816,185 +1447,189 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="41.109375" customWidth="1"/>
+    <col min="1" max="1" width="41.1047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
+      <c r="A2" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="57.6">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" ht="60" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId1" display="karthik.m+auto3@dreamorbit.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="karthik.m+auto3@dreamorbit.com"/>
+    <hyperlink ref="F2" r:id="rId2" display="karthik.m+1@dreamorbit.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.8857142857143" customWidth="1"/>
     <col min="2" max="2" width="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
-        <v>24</v>
+      <c r="A2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>27</v>
+      <c r="A3" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" display="karthik.m@dreamorbit.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="karthik.nonreg@dreamorbit.com"/>
+    <hyperlink ref="C3" r:id="rId3" display="karthik.m+81@dreamorbit.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
-        <v>44</v>
-      </c>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" display="res58@test1.com" tooltip="mailto:res58@test1.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="res897@test2.com" tooltip="mailto:res897@test2.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nov 15 from office
</commit_message>
<xml_diff>
--- a/lib/inputs.xlsx
+++ b/lib/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12600" firstSheet="6" activeTab="10"/>
+    <workbookView windowWidth="28455" windowHeight="12030" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginData" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,12 @@
     <sheet name="NonExistingResearcherEmail" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:B2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>UserName</t>
   </si>
@@ -156,16 +157,13 @@
     <t>auto111@gmail.com</t>
   </si>
   <si>
-    <t>res4@test3.com</t>
-  </si>
-  <si>
-    <t>Already existing user</t>
+    <t>res4test3.com</t>
+  </si>
+  <si>
+    <t>invalid format</t>
   </si>
   <si>
     <t>auto@hm.c</t>
-  </si>
-  <si>
-    <t>invalid format</t>
   </si>
   <si>
     <t>*****</t>
@@ -176,10 +174,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -214,6 +212,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -222,17 +241,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -244,6 +256,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -251,92 +304,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,6 +325,35 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -366,25 +364,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,157 +544,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,26 +555,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -591,6 +569,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,17 +597,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,6 +623,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -649,159 +641,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1172,8 +1170,8 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1202,7 +1200,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1210,12 +1208,12 @@
         <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="res4@test3.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="res4test3.com"/>
     <hyperlink ref="A3" r:id="rId2" display="auto@hm.c" tooltip="mailto:auto@hm.c"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1228,7 +1226,7 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1244,7 +1242,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On 25 nov from office
</commit_message>
<xml_diff>
--- a/lib/inputs.xlsx
+++ b/lib/inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28455" windowHeight="12030" firstSheet="6" activeTab="9"/>
+    <workbookView windowWidth="28455" windowHeight="12015" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginData" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ValidResearcherEmails" sheetId="9" r:id="rId9"/>
     <sheet name="InvalidResearcherEmails" sheetId="10" r:id="rId10"/>
     <sheet name="NonExistingResearcherEmail" sheetId="11" r:id="rId11"/>
+    <sheet name="ScheduleNotification" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:B2"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
   <si>
     <t>UserName</t>
   </si>
@@ -167,6 +168,24 @@
   </si>
   <si>
     <t>*****</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>6 Minute Walk Test</t>
+  </si>
+  <si>
+    <t>Daily</t>
   </si>
 </sst>
 </file>
@@ -174,10 +193,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -212,6 +231,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -219,22 +267,70 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,108 +344,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,6 +383,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -382,169 +521,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,16 +578,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,6 +619,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -607,36 +635,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -655,151 +663,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1170,7 +1189,7 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1243,6 +1262,49 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="23.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="15.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>